<commit_message>
second commit - some corrections and updates
</commit_message>
<xml_diff>
--- a/media/timetable/blank.xlsx
+++ b/media/timetable/blank.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\FrostHack\Project\media\timetable_excel_file\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\FrostHack\Project\media\timetable\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{EE5AB0A4-5B2D-4FDE-876E-381A86415DCA}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C86693A0-ED89-4647-9AAB-9A04F6D2ED33}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="735" yWindow="735" windowWidth="14550" windowHeight="10125" xr2:uid="{42F21FE2-4358-4FBD-A17C-BDC9BC51D379}"/>
+    <workbookView xWindow="390" yWindow="390" windowWidth="14550" windowHeight="10125" xr2:uid="{42F21FE2-4358-4FBD-A17C-BDC9BC51D379}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>9: 00 - 9:50</t>
   </si>
@@ -73,6 +73,9 @@
   </si>
   <si>
     <t>updated</t>
+  </si>
+  <si>
+    <t>Days</t>
   </si>
 </sst>
 </file>
@@ -427,13 +430,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7F436DBF-FED7-44CD-9F7B-2542594AF2EF}">
   <dimension ref="A1:F6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I7" sqref="I7"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>13</v>
+      </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>

</xml_diff>